<commit_message>
Adding 5 Binary Tree Questions
</commit_message>
<xml_diff>
--- a/List of questions.xlsx
+++ b/List of questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\BTech\semester4\450 dsa questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86F751E-2B3B-4D73-878A-5F8C64BF09FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266388F5-84E9-4AFD-AF23-990426D71A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="540">
   <si>
     <t>Topic:</t>
   </si>
@@ -1639,6 +1639,12 @@
   </si>
   <si>
     <t>my first intution is wrong</t>
+  </si>
+  <si>
+    <t>took hint</t>
+  </si>
+  <si>
+    <t>impo, good use of hashing</t>
   </si>
 </sst>
 </file>
@@ -2174,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B115" zoomScale="70" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="70" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2203,7 +2209,7 @@
       </c>
       <c r="E2" s="7">
         <f>SUM(F6:F481)</f>
-        <v>306</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="29.4">
@@ -2212,11 +2218,11 @@
       </c>
       <c r="E3" s="7">
         <f>2*E2/9</f>
-        <v>68</v>
+        <v>69.111111111111114</v>
       </c>
       <c r="F3" s="4">
         <f>COUNT(F6:F481)</f>
-        <v>306</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="21">
@@ -5304,8 +5310,11 @@
       <c r="C197" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D197" s="18" t="s">
-        <v>3</v>
+      <c r="D197" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="F197" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="21">
@@ -5318,8 +5327,11 @@
       <c r="C198" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D198" s="18" t="s">
-        <v>3</v>
+      <c r="D198" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="F198" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="21">
@@ -5332,8 +5344,11 @@
       <c r="C199" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D199" s="18" t="s">
-        <v>3</v>
+      <c r="D199" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="F199" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:6" ht="21">
@@ -5346,8 +5361,14 @@
       <c r="C200" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="D200" s="18" t="s">
-        <v>3</v>
+      <c r="D200" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="F200" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="21">
@@ -5360,8 +5381,14 @@
       <c r="C201" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D201" s="18" t="s">
-        <v>3</v>
+      <c r="D201" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="F201" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:6" ht="21">

</xml_diff>